<commit_message>
Updated data clumn labels and created .xlsx and .csv files for strat section with individual samples.
</commit_message>
<xml_diff>
--- a/data/Excel/Sinclair 2011-2012.xlsx
+++ b/data/Excel/Sinclair 2011-2012.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jepanzik/Documents/Research/Panzik et al. 2015 (Sinclair)/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jepanzik/Documents/Research/Paleomag/2016 Panzik et al. (Sinclair)/data/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25C4371-1D96-CD44-845A-03B2A867082E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C04750-623E-B74C-BBC4-0753E83E67B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40" yWindow="580" windowWidth="27640" windowHeight="16540" xr2:uid="{B7DB4133-8ED6-A64D-828D-88B133B8F0A3}"/>
   </bookViews>
@@ -39,24 +39,6 @@
     <t>Site</t>
   </si>
   <si>
-    <t>Brief Description</t>
-  </si>
-  <si>
-    <t>Site Latitude (°N)</t>
-  </si>
-  <si>
-    <t>Site Longitude (°E)</t>
-  </si>
-  <si>
-    <t>a-95 (°)</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>JP1101</t>
   </si>
   <si>
@@ -411,18 +393,6 @@
     <t>F</t>
   </si>
   <si>
-    <t>Declination (°)</t>
-  </si>
-  <si>
-    <t>Inclination (°)</t>
-  </si>
-  <si>
-    <t>Age (Ma)</t>
-  </si>
-  <si>
-    <t>Age Uncert (Ma)</t>
-  </si>
-  <si>
     <t>Formation</t>
   </si>
   <si>
@@ -430,6 +400,36 @@
   </si>
   <si>
     <t>Guperas</t>
+  </si>
+  <si>
+    <t>Brief.Desc</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>AgeUncert</t>
+  </si>
+  <si>
+    <t>Lat</t>
+  </si>
+  <si>
+    <t>Long</t>
+  </si>
+  <si>
+    <t>Dec</t>
+  </si>
+  <si>
+    <t>Inc</t>
+  </si>
+  <si>
+    <t>a95</t>
+  </si>
+  <si>
+    <t>n_Used</t>
+  </si>
+  <si>
+    <t>N_Collected</t>
   </si>
 </sst>
 </file>
@@ -784,7 +784,7 @@
   <dimension ref="A1:Q83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -811,66 +811,66 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>122</v>
       </c>
       <c r="C1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I1" t="s">
+        <v>126</v>
+      </c>
+      <c r="J1" t="s">
+        <v>111</v>
+      </c>
+      <c r="K1" t="s">
+        <v>112</v>
+      </c>
+      <c r="L1" t="s">
+        <v>127</v>
+      </c>
+      <c r="M1" t="s">
+        <v>128</v>
+      </c>
+      <c r="N1" t="s">
         <v>129</v>
       </c>
-      <c r="D1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E1" t="s">
-        <v>119</v>
-      </c>
-      <c r="F1" t="s">
-        <v>127</v>
-      </c>
-      <c r="G1" t="s">
-        <v>128</v>
-      </c>
-      <c r="H1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" t="s">
-        <v>117</v>
-      </c>
-      <c r="K1" t="s">
-        <v>118</v>
-      </c>
-      <c r="L1" t="s">
-        <v>125</v>
-      </c>
-      <c r="M1" t="s">
-        <v>126</v>
-      </c>
-      <c r="N1" t="s">
-        <v>4</v>
-      </c>
       <c r="O1" t="s">
-        <v>5</v>
+        <v>130</v>
       </c>
       <c r="P1" t="s">
-        <v>6</v>
+        <v>131</v>
       </c>
       <c r="Q1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H2">
         <v>-25.724983333333334</v>
@@ -893,16 +893,16 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H3">
         <v>-25.724983333333334</v>
@@ -913,16 +913,16 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H4">
         <v>-25.724983333333334</v>
@@ -948,19 +948,19 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="H5">
         <v>-25.725650000000002</v>
@@ -986,19 +986,19 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="H6">
         <v>-25.725650000000002</v>
@@ -1024,16 +1024,16 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H7">
         <v>-25.715050000000002</v>
@@ -1042,21 +1042,21 @@
         <v>16.618783333333333</v>
       </c>
       <c r="Q7" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H8">
         <v>-25.725650000000002</v>
@@ -1065,21 +1065,21 @@
         <v>16.595916666666668</v>
       </c>
       <c r="Q8" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H9">
         <v>-25.713383333333333</v>
@@ -1105,19 +1105,19 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E10" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="H10">
         <v>-25.713383333333333</v>
@@ -1143,19 +1143,19 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="H11">
         <v>-25.510033333333332</v>
@@ -1181,19 +1181,19 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E12" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="H12">
         <v>-25.510033333333332</v>
@@ -1219,16 +1219,16 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H13">
         <v>-25.506399999999999</v>
@@ -1254,16 +1254,16 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D14" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H14">
         <v>-25.452850000000002</v>
@@ -1289,16 +1289,16 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D15" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H15">
         <v>-25.452850000000002</v>
@@ -1324,16 +1324,16 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H16">
         <v>-25.453499999999998</v>
@@ -1356,16 +1356,16 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D17" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H17">
         <v>-25.453600000000002</v>
@@ -1391,16 +1391,16 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D18" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H18">
         <v>-25.482516666666665</v>
@@ -1423,16 +1423,16 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D19" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H19">
         <v>-25.482716666666668</v>
@@ -1455,16 +1455,16 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C20" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D20" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H20">
         <v>-25.482816666666668</v>
@@ -1490,16 +1490,16 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D21" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H21">
         <v>-25.482816666666668</v>
@@ -1525,16 +1525,16 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C22" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D22" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H22">
         <v>-25.483383333333332</v>
@@ -1560,19 +1560,19 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C23" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D23" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E23" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="H23">
         <v>-25.482966666666666</v>
@@ -1598,19 +1598,19 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C24" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D24" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E24" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="H24">
         <v>-25.482966666666666</v>
@@ -1636,16 +1636,16 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C25" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D25" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H25">
         <v>-25.482500000000002</v>
@@ -1671,16 +1671,16 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C26" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D26" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H26">
         <v>-25.482500000000002</v>
@@ -1706,16 +1706,16 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B27" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C27" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D27" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H27">
         <v>-25.482383333333335</v>
@@ -1741,16 +1741,16 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C28" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D28" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H28">
         <v>-25.482383333333335</v>
@@ -1776,16 +1776,16 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B29" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C29" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D29" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H29">
         <v>-25.482199999999999</v>
@@ -1811,16 +1811,16 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B30" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C30" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D30" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H30">
         <v>-25.482199999999999</v>
@@ -1846,16 +1846,16 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C31" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D31" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H31">
         <v>-25.483216666666667</v>
@@ -1881,16 +1881,16 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B32" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C32" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D32" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H32">
         <v>-25.482916666666668</v>
@@ -1916,16 +1916,16 @@
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B33" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C33" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D33" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H33">
         <v>-25.482916666666668</v>
@@ -1951,16 +1951,16 @@
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B34" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C34" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D34" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H34">
         <v>-25.49295</v>
@@ -1986,16 +1986,16 @@
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B35" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C35" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D35" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H35">
         <v>-25.49295</v>
@@ -2021,16 +2021,16 @@
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B36" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C36" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D36" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H36">
         <v>-25.49295</v>
@@ -2056,16 +2056,16 @@
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B37" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C37" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D37" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H37">
         <v>-25.497016666666667</v>
@@ -2091,16 +2091,16 @@
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B38" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C38" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D38" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H38">
         <v>-25.497016666666667</v>
@@ -2126,16 +2126,16 @@
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B39" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C39" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D39" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F39">
         <v>1105.22</v>
@@ -2167,16 +2167,16 @@
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B40" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C40" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D40" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F40">
         <v>1105.22</v>
@@ -2208,16 +2208,16 @@
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B41" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C41" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D41" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H41">
         <v>-25.707833333333333</v>
@@ -2243,16 +2243,16 @@
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B42" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C42" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D42" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H42">
         <v>-25.707833333333333</v>
@@ -2261,21 +2261,21 @@
         <v>16.573799999999999</v>
       </c>
       <c r="Q42" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B43" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C43" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D43" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F43">
         <v>1105.54</v>
@@ -2307,16 +2307,16 @@
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B44" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C44" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D44" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F44">
         <v>1105.54</v>
@@ -2348,16 +2348,16 @@
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B45" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C45" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D45" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H45">
         <v>-25.710316666666667</v>
@@ -2366,21 +2366,21 @@
         <v>16.680883333333334</v>
       </c>
       <c r="Q45" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B46" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C46" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D46" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H46">
         <v>-25.713000000000001</v>
@@ -2406,16 +2406,16 @@
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B47" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C47" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D47" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H47">
         <v>-25.713000000000001</v>
@@ -2441,16 +2441,16 @@
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B48" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C48" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D48" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H48">
         <v>-25.714466666666667</v>
@@ -2476,16 +2476,16 @@
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B49" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C49" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D49" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H49">
         <v>-25.714466666666667</v>
@@ -2511,19 +2511,19 @@
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B50" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C50" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D50" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E50" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="H50">
         <v>-25.714449999999999</v>
@@ -2546,19 +2546,19 @@
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B51" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C51" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D51" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E51" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="H51">
         <v>-25.714500000000001</v>
@@ -2584,19 +2584,19 @@
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B52" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C52" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D52" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E52" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="H52">
         <v>-25.714549999999999</v>
@@ -2622,16 +2622,16 @@
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B53" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C53" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D53" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H53">
         <v>-25.714466666666667</v>
@@ -2657,16 +2657,16 @@
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B54" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C54" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D54" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H54">
         <v>-25.714466666666667</v>
@@ -2692,16 +2692,16 @@
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B55" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C55" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D55" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H55">
         <v>-25.713850000000001</v>
@@ -2710,24 +2710,24 @@
         <v>16.647433333333332</v>
       </c>
       <c r="Q55" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B56" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C56" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D56" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E56" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="H56">
         <v>-25.713766666666668</v>
@@ -2753,19 +2753,19 @@
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B57" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C57" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D57" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E57" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="H57">
         <v>-25.713766666666668</v>
@@ -2791,16 +2791,16 @@
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B58" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C58" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D58" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H58">
         <v>-25.711449999999999</v>
@@ -2809,24 +2809,24 @@
         <v>16.646383333333333</v>
       </c>
       <c r="Q58" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B59" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C59" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D59" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E59" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="H59">
         <v>-25.711266666666667</v>
@@ -2852,19 +2852,19 @@
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B60" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C60" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D60" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E60" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="H60">
         <v>-25.71125</v>
@@ -2890,19 +2890,19 @@
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B61" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C61" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D61" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E61" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="H61">
         <v>-25.725619999999999</v>
@@ -2928,19 +2928,19 @@
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B62" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C62" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D62" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E62" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="H62">
         <v>-25.725940000000001</v>
@@ -2966,16 +2966,16 @@
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B63" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C63" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D63" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H63">
         <v>-25.711200000000002</v>
@@ -3001,16 +3001,16 @@
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B64" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C64" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D64" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H64">
         <v>-25.709620000000001</v>
@@ -3036,16 +3036,16 @@
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B65" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C65" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D65" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H65">
         <v>-25.71105</v>
@@ -3071,16 +3071,16 @@
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B66" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C66" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D66" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H66">
         <v>-25.711829999999999</v>
@@ -3091,16 +3091,16 @@
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B67" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C67" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D67" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E67">
         <v>1</v>
@@ -3129,16 +3129,16 @@
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B68" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C68" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="D68" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E68">
         <v>1</v>
@@ -3173,16 +3173,16 @@
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B69" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C69" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="D69" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E69">
         <v>1</v>
@@ -3214,16 +3214,16 @@
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B70" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C70" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="D70" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E70">
         <v>1</v>
@@ -3258,16 +3258,16 @@
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B71" t="s">
+        <v>92</v>
+      </c>
+      <c r="C71" t="s">
+        <v>121</v>
+      </c>
+      <c r="D71" t="s">
         <v>98</v>
-      </c>
-      <c r="C71" t="s">
-        <v>131</v>
-      </c>
-      <c r="D71" t="s">
-        <v>104</v>
       </c>
       <c r="E71">
         <v>1</v>
@@ -3302,16 +3302,16 @@
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B72" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C72" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="D72" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E72">
         <v>1</v>
@@ -3346,16 +3346,16 @@
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B73" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C73" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="D73" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E73">
         <v>2</v>
@@ -3373,21 +3373,21 @@
         <v>110</v>
       </c>
       <c r="Q73" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B74" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C74" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="D74" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E74">
         <v>2</v>
@@ -3422,16 +3422,16 @@
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B75" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C75" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="D75" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E75">
         <v>2</v>
@@ -3466,16 +3466,16 @@
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B76" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C76" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="D76" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E76">
         <v>1</v>
@@ -3510,16 +3510,16 @@
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B77" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C77" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="D77" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E77">
         <v>1</v>
@@ -3554,16 +3554,16 @@
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B78" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C78" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="D78" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E78">
         <v>2</v>
@@ -3598,16 +3598,16 @@
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B79" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C79" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="D79" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E79">
         <v>3</v>
@@ -3642,16 +3642,16 @@
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B80" t="s">
+        <v>104</v>
+      </c>
+      <c r="C80" t="s">
+        <v>121</v>
+      </c>
+      <c r="D80" t="s">
         <v>110</v>
-      </c>
-      <c r="C80" t="s">
-        <v>131</v>
-      </c>
-      <c r="D80" t="s">
-        <v>116</v>
       </c>
       <c r="E80">
         <v>4</v>
@@ -3680,16 +3680,16 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B81" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C81" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="D81" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E81">
         <v>4</v>
@@ -3703,16 +3703,16 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B82" t="s">
+        <v>104</v>
+      </c>
+      <c r="C82" t="s">
+        <v>121</v>
+      </c>
+      <c r="D82" t="s">
         <v>110</v>
-      </c>
-      <c r="C82" t="s">
-        <v>131</v>
-      </c>
-      <c r="D82" t="s">
-        <v>116</v>
       </c>
       <c r="E82">
         <v>5</v>
@@ -3726,16 +3726,16 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B83" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C83" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="D83" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E83">
         <v>5</v>

</xml_diff>